<commit_message>
Minor changes: details on the error about the package_name field, reduced timeout for the connexion test, update the Excel file (removed unnecessary lines)
</commit_message>
<xml_diff>
--- a/src/ckanapi_harvesters/builder/builder_package_example.xlsx
+++ b/src/ckanapi_harvesters/builder/builder_package_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\granierp\Projets\GPS_Mobilite_numerique\VRS_MobSciDatFactory\Repositories\ckanapi_harvesters\src\ckanapi_harvesters\builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F1942D-1C74-45D0-B7CC-FE555CF3A5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AEDD04-B05D-442B-81AC-9BD0BDE9D66C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24216" yWindow="504" windowWidth="21600" windowHeight="11232" firstSheet="2" activeTab="2" xr2:uid="{0974C446-06D1-4D56-994E-F584EC60B88C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="2" activeTab="2" xr2:uid="{0974C446-06D1-4D56-994E-F584EC60B88C}"/>
   </bookViews>
   <sheets>
     <sheet name="ckan" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="238">
   <si>
     <t>Age of the individual</t>
   </si>
@@ -116,9 +116,6 @@
     <t>text</t>
   </si>
   <si>
-    <t>Source</t>
-  </si>
-  <si>
     <t>License</t>
   </si>
   <si>
@@ -140,12 +137,6 @@
     <t>Maintainer Email</t>
   </si>
   <si>
-    <t>Algorithm</t>
-  </si>
-  <si>
-    <t>Algorithm Version</t>
-  </si>
-  <si>
     <t>Mode</t>
   </si>
   <si>
@@ -252,9 +243,6 @@
   </si>
   <si>
     <t>Title of the resource</t>
-  </si>
-  <si>
-    <t>Name used in the URL (short name)</t>
   </si>
   <si>
     <t>Private/Public</t>
@@ -571,9 +559,6 @@
     <t>Comma-separated list of tags (refer to data policy)</t>
   </si>
   <si>
-    <t>Custom key-value pair example (refer to data policy)</t>
-  </si>
-  <si>
     <t>A URL for the dataset's source</t>
   </si>
   <si>
@@ -691,9 +676,6 @@
     <t>Path to a text file containing 3 lines with the proxy authentication method, username and password, relative to this Excel workbook folder. This applies to all connexions (to CKAN server and external resources)</t>
   </si>
   <si>
-    <t>Test value</t>
-  </si>
-  <si>
     <t>Description can use Markdown formatting</t>
   </si>
   <si>
@@ -865,6 +847,9 @@
 - Ignored: the line is ignored
 - MultiFile: This manages a set of files to be uploaded as separate resources. The file names are identical to the resource names. The resource name field is only indicative. The _File/URL_ attribute can be used to specify a separate folder on your local file system, relative to the resources base directory. Specify file filters using a `glob` wildcard. The files used by single-resource lines are ignored by the wildcard selection.
 - MultiDataStore: A MultiFile which initiates a DataStore and manages field metadata. The forbidden wildcard characters in the name of the Excel spreadsheet for field metadata must be replaced by `#`.</t>
+  </si>
+  <si>
+    <t>Name identifying the dataset, used in the URL (short name, lowercase)</t>
   </si>
 </sst>
 </file>
@@ -1349,77 +1334,77 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C7" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C9" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -1446,39 +1431,39 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>3</v>
@@ -1486,582 +1471,582 @@
     </row>
     <row r="7" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C7" s="18"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>105</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C13" s="19"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C29" s="18"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C38" s="19"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="375" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C51" s="20"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C52" s="21"/>
     </row>
     <row r="53" spans="1:3" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C53" s="18"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2100,65 +2085,65 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2172,40 +2157,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C74C64-19A1-4B6C-85B0-52803ED84917}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="127" style="1" customWidth="1"/>
-    <col min="3" max="3" width="56.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="59.7109375" style="1" customWidth="1"/>
     <col min="4" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>69</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2213,10 +2198,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2224,10 +2209,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2240,21 +2225,21 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2262,78 +2247,51 @@
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>161</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2341,16 +2299,22 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{95CB3E82-6EE9-414D-954E-96F0A08C1100}">
           <x14:formula1>
             <xm:f>validation!$A$3:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B6:B7</xm:sqref>
+          <xm:sqref>B6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{68261CF8-9659-443F-886B-22139359275F}">
           <x14:formula1>
             <xm:f>validation!$A$7:$A$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6D2883CF-2C8E-4070-9517-495F6947145A}">
+          <x14:formula1>
+            <xm:f>validation!$A$7:$A$9</xm:f>
           </x14:formula1>
           <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
@@ -2390,31 +2354,31 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2425,10 +2389,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -2437,118 +2401,118 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
       </c>
       <c r="K3" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G8" t="s">
         <v>15</v>
@@ -2556,36 +2520,36 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D9" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F9" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D10" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="F10" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2627,13 +2591,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
@@ -2644,7 +2608,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -2652,10 +2616,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>0</v>
@@ -2685,13 +2649,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
@@ -2699,24 +2663,24 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2724,7 +2688,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
@@ -2738,18 +2702,18 @@
         <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2757,10 +2721,10 @@
         <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2768,21 +2732,21 @@
         <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2790,10 +2754,10 @@
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2820,13 +2784,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
@@ -2837,7 +2801,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
@@ -2845,10 +2809,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>0</v>
@@ -2878,13 +2842,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
@@ -2892,24 +2856,24 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2917,7 +2881,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
@@ -2931,18 +2895,18 @@
         <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2950,10 +2914,10 @@
         <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2961,21 +2925,21 @@
         <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2983,10 +2947,10 @@
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2998,7 +2962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397C6D0D-9607-4B06-96F5-66D1EA23B080}">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
@@ -3010,52 +2974,52 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="14"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B13" s="14"/>
     </row>
@@ -3066,7 +3030,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -3076,182 +3040,182 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B34" s="14"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B42" s="14"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B47" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B48" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B49" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B50" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B51" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B52" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B53" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B57" s="14"/>
     </row>
@@ -3260,7 +3224,7 @@
         <v>6</v>
       </c>
       <c r="B58" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -3275,17 +3239,17 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>